<commit_message>
improved map figures so that only shelf is shown, and 0 values are highlighted as warm grey. Also made figure to show differences in deltas.
</commit_message>
<xml_diff>
--- a/processed_data/table_delta_masked.xlsx
+++ b/processed_data/table_delta_masked.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr date1904="1" showInkAnnotation="0" hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3160" yWindow="4460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="3060" yWindow="5240" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="table_delta_masked.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="13">
   <si>
     <t>variable</t>
   </si>
@@ -65,8 +65,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="0.000"/>
-    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -74,7 +74,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -142,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -182,15 +181,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -204,8 +209,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="45">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -225,6 +243,9 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -244,6 +265,9 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -573,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="A1:F14"/>
+      <selection activeCell="M14" sqref="H3:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -587,25 +611,39 @@
     <col min="4" max="4" width="8.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9" t="s">
+      <c r="D1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9"/>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="11"/>
-      <c r="B2" s="10"/>
+      <c r="F1" s="12"/>
+      <c r="H1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" s="9"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
@@ -618,8 +656,22 @@
       <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="H2" s="11"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="7" t="s">
         <v>11</v>
       </c>
@@ -638,8 +690,26 @@
       <c r="F3" s="3">
         <v>44.913841987552097</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="H3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>429.986974271012</v>
+      </c>
+      <c r="K3" s="3">
+        <v>12.975398652177599</v>
+      </c>
+      <c r="L3" s="2">
+        <v>357.74533912268902</v>
+      </c>
+      <c r="M3" s="3">
+        <v>44.913841987552097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -658,8 +728,26 @@
       <c r="F4" s="4">
         <v>0.12598207569044101</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="H4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2">
+        <v>767.07028816466504</v>
+      </c>
+      <c r="K4" s="2">
+        <v>275.64234364444098</v>
+      </c>
+      <c r="L4" s="2">
+        <v>857.79165441995099</v>
+      </c>
+      <c r="M4" s="2">
+        <v>180.895548808868</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -678,8 +766,26 @@
       <c r="F5" s="4">
         <v>1.94321081991107</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="2">
+        <v>761.76583533447604</v>
+      </c>
+      <c r="K5" s="2">
+        <v>156.962807462271</v>
+      </c>
+      <c r="L5" s="2">
+        <v>665.79593705930301</v>
+      </c>
+      <c r="M5" s="2">
+        <v>101.17061206249799</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
@@ -698,8 +804,26 @@
       <c r="F6" s="4">
         <v>1.1198927425084101E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="H6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4">
+        <v>-0.43547489726689698</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.22153491530251401</v>
+      </c>
+      <c r="L6" s="4">
+        <v>-0.59948048838025803</v>
+      </c>
+      <c r="M6" s="16">
+        <v>6.8046095748164295E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -718,8 +842,26 @@
       <c r="F7" s="2">
         <v>180.895548808868</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="H7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="4">
+        <v>-0.47667281584704502</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.28990624763682299</v>
+      </c>
+      <c r="L7" s="4">
+        <v>-0.53396198044613097</v>
+      </c>
+      <c r="M7" s="16">
+        <v>7.9450764995049994E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -738,8 +880,26 @@
       <c r="F8" s="4">
         <v>0.58244117173136101</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="H8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4">
+        <v>-0.32938213475140099</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.10014751212096699</v>
+      </c>
+      <c r="L8" s="4">
+        <v>-0.40279243582639501</v>
+      </c>
+      <c r="M8" s="16">
+        <v>4.3589088430404897E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -758,8 +918,26 @@
       <c r="F9" s="4">
         <v>3.54193197765753</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="H9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="4">
+        <v>1.7334238970840401</v>
+      </c>
+      <c r="K9" s="4">
+        <v>0.63623637729175497</v>
+      </c>
+      <c r="L9" s="4">
+        <v>2.0912271464257</v>
+      </c>
+      <c r="M9" s="4">
+        <v>0.58244117173136101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
@@ -778,8 +956,26 @@
       <c r="F10" s="4">
         <v>5.7385478457604999E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="H10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="4">
+        <v>2.1025345111492202</v>
+      </c>
+      <c r="K10" s="4">
+        <v>0.48753932764591801</v>
+      </c>
+      <c r="L10" s="4">
+        <v>2.5646922220572899</v>
+      </c>
+      <c r="M10" s="4">
+        <v>0.19063560489776499</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -798,8 +994,26 @@
       <c r="F11" s="2">
         <v>101.17061206249799</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="H11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>3.1052709433962198</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.26136799485270501</v>
+      </c>
+      <c r="L11" s="4">
+        <v>2.8999236145242602</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.12598207569044101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
@@ -818,8 +1032,26 @@
       <c r="F12" s="4">
         <v>0.19063560489776499</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="H12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="4">
+        <v>-0.24995938662092601</v>
+      </c>
+      <c r="K12" s="4">
+        <v>8.1796292261151302E-2</v>
+      </c>
+      <c r="L12" s="4">
+        <v>-0.28455831292214001</v>
+      </c>
+      <c r="M12" s="4">
+        <v>5.7385478457604999E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
@@ -838,8 +1070,26 @@
       <c r="F13" s="4">
         <v>3.0335094004467398</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="H13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" s="4">
+        <v>-0.279832109777015</v>
+      </c>
+      <c r="K13" s="4">
+        <v>2.0674732466675099E-2</v>
+      </c>
+      <c r="L13" s="4">
+        <v>-0.283938265419728</v>
+      </c>
+      <c r="M13" s="4">
+        <v>1.1198927425084101E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -858,10 +1108,28 @@
       <c r="F14" s="6">
         <v>9.3862111915156404E-3</v>
       </c>
+      <c r="H14" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J14" s="6">
+        <v>-0.30577485763293299</v>
+      </c>
+      <c r="K14" s="6">
+        <v>2.87653230510619E-2</v>
+      </c>
+      <c r="L14" s="6">
+        <v>-0.31871149261485898</v>
+      </c>
+      <c r="M14" s="6">
+        <v>9.3862111915156404E-3</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A3:F14">
-    <sortCondition descending="1" ref="B3:B14"/>
+  <sortState ref="H4:M14">
+    <sortCondition descending="1" ref="M14"/>
   </sortState>
   <mergeCells count="4">
     <mergeCell ref="C1:D1"/>

</xml_diff>